<commit_message>
two models rand search, vessels data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiopisoni/school/ml/TDT4173-ML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6066C2-084A-D441-A9EC-CA6F0A2C6E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78DBA53-67DB-5446-A0FE-A738BCADCC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{D68E945C-6F27-3448-8C7F-A03AA4683781}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>file</t>
   </si>
@@ -104,9 +104,6 @@
     <t>reults_1.8</t>
   </si>
   <si>
-    <t>results_2.0</t>
-  </si>
-  <si>
     <t>72 trainig sets, scaled, not tuned</t>
   </si>
   <si>
@@ -114,6 +111,33 @@
   </si>
   <si>
     <t>72ts with hyper param of 18ts  and added features (port coord, dayofweek, uncertain rot)</t>
+  </si>
+  <si>
+    <t>"", 3days means, time to eta in seconds</t>
+  </si>
+  <si>
+    <t>60ts, ""</t>
+  </si>
+  <si>
+    <t>72ts, isMoored</t>
+  </si>
+  <si>
+    <t>result_2.3</t>
+  </si>
+  <si>
+    <t>result_2.2</t>
+  </si>
+  <si>
+    <t>result_2.1</t>
+  </si>
+  <si>
+    <t>result_2.0</t>
+  </si>
+  <si>
+    <t>sudo apt install git-lfs</t>
+  </si>
+  <si>
+    <t>git lfs install</t>
   </si>
 </sst>
 </file>
@@ -155,9 +179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74932C60-FA87-D240-BAA8-EDFF9D1DF015}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,9 +530,10 @@
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="82.6640625" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -533,7 +561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -547,7 +575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -561,7 +589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -575,7 +603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>0.65091458396108304</v>
       </c>
@@ -583,7 +611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -597,7 +625,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -608,10 +636,10 @@
         <v>124.13005</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -625,7 +653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -633,7 +661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -644,12 +672,12 @@
         <v>121.16776</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1">
         <v>0.83049377523877899</v>
@@ -658,7 +686,55 @@
         <v>114.25762</v>
       </c>
       <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.76579529521828305</v>
+      </c>
+      <c r="C13" s="1">
+        <v>102.74959</v>
+      </c>
+      <c r="D13" t="s">
         <v>25</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.65849783034842602</v>
+      </c>
+      <c r="C14" s="2">
+        <v>103.86183</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.77123279476968698</v>
+      </c>
+      <c r="C15" s="2">
+        <v>101.11895</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
project folder with short notebooks
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiopisoni/school/ml/TDT4173-ML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2253D109-6489-6444-9AAA-5C69A9965763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D35096D-C89E-4842-8351-CA0EB83F7D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{D68E945C-6F27-3448-8C7F-A03AA4683781}"/>
   </bookViews>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74932C60-FA87-D240-BAA8-EDFF9D1DF015}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>